<commit_message>
lift with two slats
</commit_message>
<xml_diff>
--- a/torgues.xlsx
+++ b/torgues.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="19095" windowHeight="8460" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="48" windowWidth="16608" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Servos" sheetId="1" r:id="rId1"/>
     <sheet name="Motor" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>bucket</t>
   </si>
@@ -27,18 +27,9 @@
     <t>K</t>
   </si>
   <si>
-    <t>bucket servo</t>
-  </si>
-  <si>
-    <t>lever for bucket servo,cm</t>
-  </si>
-  <si>
     <t>weight, g</t>
   </si>
   <si>
-    <t>lever for cover servo,cm</t>
-  </si>
-  <si>
     <t>cover servo</t>
   </si>
   <si>
@@ -48,15 +39,9 @@
     <t>cover</t>
   </si>
   <si>
-    <t>beams for mount cover</t>
-  </si>
-  <si>
     <t>torque, kg*cm</t>
   </si>
   <si>
-    <t>levr foe turn bucket servo</t>
-  </si>
-  <si>
     <t>arm of force, cm</t>
   </si>
   <si>
@@ -66,9 +51,6 @@
     <t>servo bucket to side</t>
   </si>
   <si>
-    <t>chain</t>
-  </si>
-  <si>
     <t>servo cover</t>
   </si>
   <si>
@@ -79,6 +61,21 @@
   </si>
   <si>
     <t>moment</t>
+  </si>
+  <si>
+    <t>arm of force for cover servo,cm</t>
+  </si>
+  <si>
+    <t>arm of force for bucket servo,cm</t>
+  </si>
+  <si>
+    <t>arm of force for servo that turn bucket to side</t>
+  </si>
+  <si>
+    <t>bucket up-down servo</t>
+  </si>
+  <si>
+    <t>bucket to side servo</t>
   </si>
 </sst>
 </file>
@@ -419,23 +416,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -443,24 +440,21 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>50</v>
@@ -477,16 +471,16 @@
       <c r="F2">
         <v>57</v>
       </c>
-      <c r="G2">
-        <v>33</v>
-      </c>
       <c r="H2">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>9.5</v>
@@ -503,83 +497,77 @@
       <c r="F3">
         <v>18</v>
       </c>
-      <c r="G3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F4">
-        <v>14</v>
-      </c>
-      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <f>B3+$J$2</f>
+        <v>14.3</v>
+      </c>
+      <c r="C5">
+        <f>C3+$J$2</f>
+        <v>14.3</v>
+      </c>
+      <c r="D5">
+        <f>D3+$J$2</f>
+        <v>10.399999999999999</v>
+      </c>
+      <c r="E5">
+        <f>E3+$J$2</f>
+        <v>14.3</v>
+      </c>
+      <c r="F5">
+        <f>F3+$J$2</f>
+        <v>22.8</v>
+      </c>
+      <c r="G5">
+        <f>G3+$J$2</f>
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <f>(B2*B3 + C2*C3+D2*D3+E2*E3+F2*F3+G2*G3) * H2/1000</f>
-        <v>7.4322000000000008</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6.8877000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <f>(F2*F4+G2*G4)*H2/1000</f>
-        <v>1.5435000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f>(B2*B12+C2*C12+D2*D12+E2*E12+F2*F12+G2*G12 + E6*E10) * H2 / 1000</f>
-        <v>11.413799999999998</v>
-      </c>
-      <c r="E10">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="J8">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <f>B3+$E$6</f>
-        <v>14.3</v>
-      </c>
-      <c r="C12">
-        <f>C3+$E$6</f>
-        <v>14.3</v>
-      </c>
-      <c r="D12">
-        <f>D3+$E$6</f>
-        <v>10.399999999999999</v>
-      </c>
-      <c r="E12">
-        <f>E3+$E$6</f>
-        <v>14.3</v>
-      </c>
-      <c r="F12">
-        <f t="shared" ref="F12:G12" si="0">F3+$E$6</f>
-        <v>22.8</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>15.8</v>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <f>(B2*B5+C2*C5+D2*D5+E2*E5+F2*F5+G2*G5 + J2*J8) * H2 / 1000</f>
+        <v>10.6317</v>
       </c>
     </row>
   </sheetData>
@@ -589,21 +577,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -611,30 +600,27 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>50</v>
@@ -655,18 +641,15 @@
         <v>50</v>
       </c>
       <c r="H2">
-        <v>50</v>
-      </c>
-      <c r="I2">
         <v>900</v>
       </c>
-      <c r="K2">
+      <c r="J2">
         <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>70</v>
@@ -681,25 +664,22 @@
         <v>52.5</v>
       </c>
       <c r="F3">
-        <v>61.25</v>
+        <v>62.5</v>
       </c>
       <c r="G3">
-        <v>62.5</v>
+        <v>70</v>
       </c>
       <c r="H3">
-        <v>70</v>
-      </c>
-      <c r="I3">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B6">
-        <f>(B2*B3+C2*C3+D2*D3+E2*E3+F2*F3+G2*G3+H2*H3+I2*I3) * K2 / 1000</f>
-        <v>102.46875</v>
+        <f>(B2*B3+C2*C3+D2*D3+E2*E3+F2*F3+G2*G3+H2*H3) * J2 / 1000</f>
+        <v>97.875</v>
       </c>
     </row>
   </sheetData>
@@ -713,7 +693,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>